<commit_message>
feat: navigates subrecord and edits sheets
</commit_message>
<xml_diff>
--- a/accessdb/famSheets/1 Arackaparambil.xlsx
+++ b/accessdb/famSheets/1 Arackaparambil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Workspace\GitHub\cbcefdb\accessdb\famSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32C430A6-E98F-47A4-93CF-3F58B7EC4B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C91B04E3-657F-4123-9726-EED1909710AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1530" yWindow="1515" windowWidth="21600" windowHeight="11295" xr2:uid="{691864EF-CD39-4A4F-A743-1915A8367D6B}"/>
   </bookViews>
@@ -460,7 +460,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="102">
   <si>
     <t xml:space="preserve">ക്രിസ്ത്യന്‍ ബ്രദറണ്‍ ചര്‍ച്ച് ഈസ്റ്റ് ഫോര്‍ട്ട്‌ </t>
   </si>
@@ -690,6 +690,9 @@
     <t>Own</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>Arackaparambil (H)</t>
   </si>
   <si>
@@ -736,6 +739,33 @@
   </si>
   <si>
     <t>enhetn</t>
+  </si>
+  <si>
+    <t>Ammini Jayarson</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Wife</t>
+  </si>
+  <si>
+    <t>25-09-2021</t>
+  </si>
+  <si>
+    <t>Home Maker</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
+  </si>
+  <si>
+    <t>jayarson@gmail.com</t>
+  </si>
+  <si>
+    <t>Abraham Chacko</t>
+  </si>
+  <si>
+    <t>Thankamma Chacko</t>
   </si>
 </sst>
 </file>
@@ -836,13 +866,13 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1" tint="0.249977111117893"/>
+      <color theme="0"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
-      <color theme="0"/>
+      <color theme="1" tint="0.34998626667073579"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -950,17 +980,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1532,7 +1562,7 @@
   <dimension ref="A1:I1018"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:G2"/>
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1619,31 +1649,31 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="I8" s="26" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1654,17 +1684,17 @@
       <c r="B9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
+      <c r="D9" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
     </row>
     <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19">
@@ -1673,17 +1703,17 @@
       <c r="B10" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
+      <c r="D10" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
     </row>
     <row r="11" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19">
@@ -1692,17 +1722,17 @@
       <c r="B11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
+      <c r="D11" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
     </row>
     <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="19">
@@ -1715,13 +1745,13 @@
         <v>25204</v>
       </c>
       <c r="D12" s="31">
-        <v>25204</v>
-      </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
+        <v>26579</v>
+      </c>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
     </row>
     <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19">
@@ -1730,17 +1760,17 @@
       <c r="B13" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
     </row>
     <row r="14" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="19">
@@ -1755,11 +1785,11 @@
       <c r="D14" s="31">
         <v>35208</v>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
     </row>
     <row r="15" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19">
@@ -1768,17 +1798,17 @@
       <c r="B15" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="27">
         <v>1984</v>
       </c>
-      <c r="D15" s="29">
-        <v>1984</v>
-      </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
+      <c r="D15" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
     </row>
     <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19">
@@ -1787,17 +1817,17 @@
       <c r="B16" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
     </row>
     <row r="17" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19">
@@ -1806,17 +1836,17 @@
       <c r="B17" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
+      <c r="D17" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
     </row>
     <row r="18" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19">
@@ -1825,17 +1855,17 @@
       <c r="B18" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
+      <c r="D18" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
     </row>
     <row r="19" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19">
@@ -1844,17 +1874,17 @@
       <c r="B19" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
     </row>
     <row r="20" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19">
@@ -1863,17 +1893,15 @@
       <c r="B20" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="29">
+      <c r="C20" s="27">
         <v>16513216513161</v>
       </c>
-      <c r="D20" s="29">
-        <v>16513216513161</v>
-      </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
     </row>
     <row r="21" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="19">
@@ -1882,17 +1910,17 @@
       <c r="B21" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="29">
+      <c r="C21" s="27">
         <v>8281873512</v>
       </c>
-      <c r="D21" s="29">
-        <v>8281873512</v>
-      </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
+      <c r="D21" s="27">
+        <v>9446391412</v>
+      </c>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
     </row>
     <row r="22" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="19">
@@ -1901,17 +1929,17 @@
       <c r="B22" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
+      <c r="D22" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
     </row>
     <row r="23" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19">
@@ -1920,17 +1948,17 @@
       <c r="B23" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
     </row>
     <row r="24" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="19">
@@ -1939,132 +1967,132 @@
       <c r="B24" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="29">
-        <v>-1</v>
-      </c>
-      <c r="D24" s="29">
-        <v>-1</v>
-      </c>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
+      <c r="C24" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
     </row>
     <row r="25" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="19"/>
       <c r="B25" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
     </row>
     <row r="26" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19"/>
       <c r="B26" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="D26" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
     </row>
     <row r="27" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="19"/>
       <c r="B27" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
+      <c r="C27" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
     </row>
     <row r="28" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="19"/>
       <c r="B28" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
+      <c r="C28" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
     </row>
     <row r="29" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="19"/>
       <c r="B29" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
+      <c r="C29" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
     </row>
     <row r="30" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="19"/>
       <c r="B30" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
+      <c r="C30" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
     </row>
     <row r="31" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="19"/>
       <c r="B31" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
+      <c r="C31" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
     </row>
     <row r="32" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="19">
@@ -2073,17 +2101,17 @@
       <c r="B32" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
+      <c r="C32" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
     </row>
     <row r="33" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A33" s="19">
@@ -2092,17 +2120,15 @@
       <c r="B33" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
+      <c r="C33" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
     </row>
     <row r="34" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="19">
@@ -2111,17 +2137,17 @@
       <c r="B34" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="D34" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="29"/>
+      <c r="C34" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
     </row>
     <row r="35" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A35" s="19">
@@ -2130,28 +2156,26 @@
       <c r="B35" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="D35" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
+      <c r="C35" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
     </row>
     <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
     </row>
     <row r="37" spans="1:9" ht="84.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="19">
@@ -2160,17 +2184,15 @@
       <c r="B37" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="D37" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
+      <c r="C37" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
     </row>
     <row r="38" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="19">
@@ -2179,17 +2201,15 @@
       <c r="B38" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="D38" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
+      <c r="C38" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
     </row>
     <row r="39" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="19">
@@ -2198,17 +2218,15 @@
       <c r="B39" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="D39" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="29"/>
+      <c r="C39" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
     </row>
     <row r="40" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="19">
@@ -2217,17 +2235,15 @@
       <c r="B40" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="D40" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
+      <c r="C40" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
     </row>
     <row r="41" spans="1:9" ht="84.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="19">
@@ -2236,17 +2252,15 @@
       <c r="B41" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="D41" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="29"/>
+      <c r="C41" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
     </row>
     <row r="42" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="19">
@@ -2255,17 +2269,15 @@
       <c r="B42" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
+      <c r="C42" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
     </row>
     <row r="43" spans="1:9" ht="84.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="19">
@@ -2274,17 +2286,15 @@
       <c r="B43" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="D43" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
+      <c r="C43" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
     </row>
     <row r="44" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="19">
@@ -2293,78 +2303,78 @@
       <c r="B44" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
     </row>
     <row r="45" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="19"/>
       <c r="B45" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
     </row>
     <row r="46" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="19"/>
       <c r="B46" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="29"/>
-      <c r="H46" s="29"/>
-      <c r="I46" s="29"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
     </row>
     <row r="47" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="19"/>
       <c r="B47" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="29"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="27"/>
     </row>
     <row r="48" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="19"/>
       <c r="B48" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="29"/>
-      <c r="H48" s="29"/>
-      <c r="I48" s="29"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="27"/>
     </row>
     <row r="49" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="19"/>
       <c r="B49" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="29"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="29"/>
-      <c r="I49" s="29"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="27"/>
     </row>
     <row r="50" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="19">
@@ -2373,13 +2383,13 @@
       <c r="B50" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="27"/>
     </row>
     <row r="51" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
@@ -2405,7 +2415,7 @@
     </row>
     <row r="53" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
-      <c r="B53" s="27" t="s">
+      <c r="B53" s="28" t="s">
         <v>47</v>
       </c>
       <c r="C53" s="7"/>
@@ -2472,7 +2482,7 @@
     </row>
     <row r="59" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="13"/>
-      <c r="B59" s="26" t="s">
+      <c r="B59" s="29" t="s">
         <v>52</v>
       </c>
       <c r="C59" s="8"/>
@@ -2483,7 +2493,7 @@
       <c r="I59" s="8"/>
     </row>
     <row r="60" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="26" t="s">
+      <c r="B60" s="29" t="s">
         <v>63</v>
       </c>
       <c r="C60" s="8"/>
@@ -2494,7 +2504,7 @@
       <c r="I60" s="8"/>
     </row>
     <row r="61" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="26" t="s">
+      <c r="B61" s="29" t="s">
         <v>53</v>
       </c>
       <c r="C61" s="8"/>
@@ -2505,7 +2515,7 @@
       <c r="I61" s="8"/>
     </row>
     <row r="62" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="26" t="s">
+      <c r="B62" s="29" t="s">
         <v>54</v>
       </c>
       <c r="C62" s="8"/>

</xml_diff>